<commit_message>
Flujo de caja penca pero bueh
</commit_message>
<xml_diff>
--- a/docs/flujo-cmh.xlsx
+++ b/docs/flujo-cmh.xlsx
@@ -9,15 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="costos variables" sheetId="1" r:id="rId1"/>
-    <sheet name="flujo de caja" sheetId="3" r:id="rId2"/>
+    <sheet name="inversion inicial" sheetId="7" r:id="rId1"/>
+    <sheet name="ingreso por ahorro" sheetId="1" r:id="rId2"/>
+    <sheet name="costo fijo" sheetId="6" r:id="rId3"/>
+    <sheet name="flujo de caja" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Costo mensual</t>
   </si>
@@ -123,30 +122,12 @@
     <t>Proceso</t>
   </si>
   <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>Costo variable</t>
-  </si>
-  <si>
     <t>Ingreso operacional</t>
   </si>
   <si>
-    <t>venta activo</t>
-  </si>
-  <si>
-    <t>costo variable</t>
-  </si>
-  <si>
     <t>costo fijo</t>
   </si>
   <si>
-    <t>depreciación</t>
-  </si>
-  <si>
-    <t>valor libro</t>
-  </si>
-  <si>
     <t>utilidad bruta</t>
   </si>
   <si>
@@ -156,12 +137,6 @@
     <t>inversión fija</t>
   </si>
   <si>
-    <t>capital de trabajo</t>
-  </si>
-  <si>
-    <t>valor desecho</t>
-  </si>
-  <si>
     <t>flujo</t>
   </si>
   <si>
@@ -171,27 +146,53 @@
     <t>IVA</t>
   </si>
   <si>
-    <t>Cantidad de atenciones realizadas</t>
-  </si>
-  <si>
-    <t>Costo promedio por atención</t>
-  </si>
-  <si>
-    <t>Total de atenciones realizadas</t>
-  </si>
-  <si>
-    <t>Precio promedio</t>
+    <t>Total ahorro</t>
+  </si>
+  <si>
+    <t>Amazon AWS EC2</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>Amazon AWS RDS</t>
+  </si>
+  <si>
+    <t>Desarrollo software</t>
+  </si>
+  <si>
+    <t>Implantación</t>
+  </si>
+  <si>
+    <t>Capacitación operador</t>
+  </si>
+  <si>
+    <t>Capacitación médico</t>
+  </si>
+  <si>
+    <t>Capacitación jefe de operadores</t>
+  </si>
+  <si>
+    <t>Capacitación efermero</t>
+  </si>
+  <si>
+    <t>Capacitación tecnólogo</t>
+  </si>
+  <si>
+    <t>Costo del sistema</t>
+  </si>
+  <si>
+    <t>Payback</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_(&quot;CLP&quot;* #,##0_);_(&quot;CLP&quot;* \(#,##0\);_(&quot;CLP&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -225,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -339,6 +340,43 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -364,19 +402,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -390,29 +428,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ej1"/>
-      <sheetName val="ej2"/>
-      <sheetName val="detalle ej2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="34">
-          <cell r="G34">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,15 +693,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1">
+        <v>13416000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1">
+        <f>13000*8</f>
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1">
+        <f>'ingreso por ahorro'!C26/20</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1">
+        <f>'ingreso por ahorro'!C25/20</f>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
+        <f>'ingreso por ahorro'!C28/20</f>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1">
+        <f>'ingreso por ahorro'!C33/20</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1">
+        <f>'ingreso por ahorro'!C32/20</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1">
+        <f>SUM(B2:B9)</f>
+        <v>13695000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="110" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -1228,7 +1333,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="21" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="1">
@@ -1237,17 +1342,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19">
-        <v>95</v>
-      </c>
+      <c r="A19" s="21"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1255,10 +1353,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="27">
-        <f>I18/I19</f>
-        <v>33245.614035087718</v>
-      </c>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
@@ -1824,7 +1919,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="21" t="s">
         <v>25</v>
       </c>
       <c r="I40" s="1">
@@ -1833,17 +1928,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41">
-        <v>95</v>
-      </c>
+      <c r="A41" s="21"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1851,10 +1939,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="27">
-        <f>I40/I41</f>
-        <v>4730.9941520467837</v>
-      </c>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
@@ -1868,647 +1953,523 @@
       <c r="I43" s="16"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="29"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="24"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="1">
+        <f>I18-I40</f>
+        <v>2708888.888888889</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1">
+        <f>15*670</f>
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <f>25*670</f>
+        <v>16750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
+        <f>SUM(B2:B4)</f>
+        <v>26800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="D1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="E1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="F1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="G1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="H1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="I1" s="17">
-        <v>50000</v>
-      </c>
-      <c r="J1" s="17">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="17"/>
-      <c r="C2" s="18">
-        <v>95</v>
-      </c>
-      <c r="D2" s="18">
-        <v>95</v>
-      </c>
-      <c r="E2" s="18">
-        <v>95</v>
-      </c>
-      <c r="F2" s="18">
-        <v>95</v>
-      </c>
-      <c r="G2" s="18">
-        <v>95</v>
-      </c>
-      <c r="H2" s="18">
-        <v>95</v>
-      </c>
-      <c r="I2" s="18">
-        <v>95</v>
-      </c>
-      <c r="J2" s="18">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="D2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="E2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="F2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="G2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="H2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="I2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="J2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="K2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="L2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="M2" s="17">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+      <c r="N2" s="18">
+        <f>'ingreso por ahorro'!I46</f>
+        <v>2708888.888888889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="D3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="E3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="F3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="G3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="H3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="I3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-      <c r="J3" s="17">
-        <f>'costos variables'!I20</f>
-        <v>33245.614035087718</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="D3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="E3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="F3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="G3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="H3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="I3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="J3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="K3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="L3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="M3" s="19">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+      <c r="N3" s="9">
+        <f>'costo fijo'!B5</f>
+        <v>26800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="C4" s="17">
+        <f>SUM(C2:C3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="D4" s="17">
+        <f>SUM(D2:D3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="E4" s="17">
+        <f>SUM(E2:E3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="F4" s="17">
+        <f>SUM(F2:F3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="G4" s="17">
+        <f>SUM(G2:G3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="H4" s="17">
+        <f>SUM(H2:H3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="I4" s="17">
+        <f>SUM(I2:I3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="J4" s="17">
+        <f>SUM(J2:J3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="K4" s="17">
+        <f>SUM(K2:K3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="L4" s="17">
+        <f>SUM(L2:L3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="M4" s="17">
+        <f>SUM(M2:M3)</f>
+        <v>2735688.888888889</v>
+      </c>
+      <c r="N4" s="18">
+        <f>SUM(N2:N3)</f>
+        <v>2735688.888888889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19">
+        <f>-C4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="D5" s="19">
+        <f>-D4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="E5" s="19">
+        <f>-E4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="F5" s="19">
+        <f>-F4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="G5" s="19">
+        <f>-G4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="H5" s="19">
+        <f>-H4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="I5" s="19">
+        <f>-I4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="J5" s="19">
+        <f>-J4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="K5" s="19">
+        <f>-K4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="L5" s="19">
+        <f>-L4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="M5" s="19">
+        <f>-M4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+      <c r="N5" s="9">
+        <f>-N4*B11</f>
+        <v>-519780.88888888893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17">
+        <f>C4+C5</f>
+        <v>2215908</v>
+      </c>
+      <c r="D6" s="17">
+        <f>D4+D5</f>
+        <v>2215908</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" ref="E6:J6" si="0">E4+E5</f>
+        <v>2215908</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>2215908</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>2215908</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="0"/>
+        <v>2215908</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" si="0"/>
+        <v>2215908</v>
+      </c>
+      <c r="J6" s="17">
+        <f t="shared" si="0"/>
+        <v>2215908</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" ref="K6:L6" si="1">K4+K5</f>
+        <v>2215908</v>
+      </c>
+      <c r="L6" s="17">
+        <f t="shared" si="1"/>
+        <v>2215908</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" ref="M6:N6" si="2">M4+M5</f>
+        <v>2215908</v>
+      </c>
+      <c r="N6" s="18">
+        <f t="shared" si="2"/>
+        <v>2215908</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="20">
+        <f>-'inversion inicial'!B10</f>
+        <v>-13695000</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>6</v>
-      </c>
-      <c r="I5" s="2">
-        <v>7</v>
-      </c>
-      <c r="J5" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19">
-        <f>C1*C2</f>
-        <v>4750000</v>
-      </c>
-      <c r="D6" s="19">
-        <f t="shared" ref="D6:J6" si="0">D1*D2</f>
-        <v>4750000</v>
-      </c>
-      <c r="E6" s="19">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-      <c r="F6" s="19">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-      <c r="G6" s="19">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-      <c r="H6" s="19">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-      <c r="I6" s="19">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-      <c r="J6" s="20">
-        <f t="shared" si="0"/>
-        <v>4750000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22">
-        <v>0</v>
-      </c>
-      <c r="D7" s="21">
-        <v>0</v>
-      </c>
-      <c r="E7" s="21">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21">
-        <v>0</v>
-      </c>
-      <c r="H7" s="21">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21">
-        <f>C3*C2</f>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="D8" s="21">
-        <f>D3*D2</f>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="E8" s="21">
-        <f t="shared" ref="E8:J8" si="1">E3*E2</f>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="F8" s="21">
-        <f t="shared" si="1"/>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="G8" s="21">
-        <f t="shared" si="1"/>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="H8" s="21">
-        <f t="shared" si="1"/>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="I8" s="21">
-        <f t="shared" si="1"/>
-        <v>3158333.333333333</v>
-      </c>
-      <c r="J8" s="9">
-        <f t="shared" si="1"/>
-        <v>3158333.333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21">
-        <f>-'[1]detalle ej2'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="21">
-        <f>-'[1]detalle ej2'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="21">
-        <f>-'[1]detalle ej2'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="21">
-        <f>-'[1]detalle ej2'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="21">
-        <f>-'[1]detalle ej2'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="21">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B8" s="26">
+        <f>SUM(B6:B7)</f>
+        <v>-13695000</v>
+      </c>
+      <c r="C8" s="26">
+        <f>SUM(C6:C7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="D8" s="26">
+        <f>SUM(D6:D7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="E8" s="26">
+        <f>SUM(E6:E7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="F8" s="26">
+        <f>SUM(F6:F7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="G8" s="26">
+        <f>SUM(G6:G7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="H8" s="26">
+        <f>SUM(H6:H7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="I8" s="26">
+        <f>SUM(I6:I7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="J8" s="26">
+        <f>SUM(J6:J7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="K8" s="26">
+        <f>SUM(K6:K7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="L8" s="26">
+        <f>SUM(L6:L7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="M8" s="26">
+        <f>SUM(M6:M7)</f>
+        <v>2215908</v>
+      </c>
+      <c r="N8" s="27">
+        <f>SUM(N6:N7)</f>
+        <v>2215908</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21">
-        <v>0</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0</v>
-      </c>
-      <c r="E10" s="21">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21">
-        <f>-'[1]detalle ej2'!G34</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <f>NPV(10%,B8:N8)</f>
+        <v>1275922.0180825274</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23">
-        <f>SUM(C10:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19">
-        <f>SUM(C6:C11)</f>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="D12" s="19">
-        <f t="shared" ref="D12:J12" si="2">SUM(D6:D11)</f>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="E12" s="19">
-        <f t="shared" si="2"/>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="F12" s="19">
-        <f>SUM(F6:F11)</f>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="G12" s="19">
-        <f t="shared" si="2"/>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="H12" s="19">
-        <f t="shared" si="2"/>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="I12" s="19">
-        <f t="shared" si="2"/>
-        <v>7908333.333333333</v>
-      </c>
-      <c r="J12" s="19">
-        <f t="shared" si="2"/>
-        <v>7908333.333333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23">
-        <f>-C12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="D13" s="23">
-        <f>-D12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="E13" s="23">
-        <f>-E12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="F13" s="23">
-        <f>-F12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="G13" s="23">
-        <f>-G12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="H13" s="23">
-        <f>-H12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="I13" s="23">
-        <f>-I12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-      <c r="J13" s="23">
-        <f>-J12*B23</f>
-        <v>-1502583.3333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19">
-        <f>C12+C13</f>
-        <v>6405750</v>
-      </c>
-      <c r="D14" s="19">
-        <f>D12+D13</f>
-        <v>6405750</v>
-      </c>
-      <c r="E14" s="19">
-        <f t="shared" ref="E14:J14" si="3">E12+E13</f>
-        <v>6405750</v>
-      </c>
-      <c r="F14" s="19">
-        <f t="shared" si="3"/>
-        <v>6405750</v>
-      </c>
-      <c r="G14" s="19">
-        <f t="shared" si="3"/>
-        <v>6405750</v>
-      </c>
-      <c r="H14" s="19">
-        <f t="shared" si="3"/>
-        <v>6405750</v>
-      </c>
-      <c r="I14" s="19">
-        <f t="shared" si="3"/>
-        <v>6405750</v>
-      </c>
-      <c r="J14" s="19">
-        <f t="shared" si="3"/>
-        <v>6405750</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21">
-        <f>-C10</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="21">
-        <f t="shared" ref="D15:G15" si="4">-D10</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="21">
-        <f>-H10</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="21">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21">
-        <f>SUM(C15:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="21">
-        <f>-'[1]detalle ej2'!E12</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21">
-        <v>0</v>
-      </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="21">
-        <v>0</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="19">
-        <f>SUM(B14:B19)</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="19">
-        <f>SUM(C14:C19)</f>
-        <v>6405750</v>
-      </c>
-      <c r="D20" s="19">
-        <f>SUM(D14:D19)</f>
-        <v>6405750</v>
-      </c>
-      <c r="E20" s="19">
-        <f t="shared" ref="E20:J20" si="5">SUM(E14:E19)</f>
-        <v>6405750</v>
-      </c>
-      <c r="F20" s="19">
-        <f t="shared" si="5"/>
-        <v>6405750</v>
-      </c>
-      <c r="G20" s="19">
-        <f t="shared" si="5"/>
-        <v>6405750</v>
-      </c>
-      <c r="H20" s="19">
-        <f t="shared" si="5"/>
-        <v>6405750</v>
-      </c>
-      <c r="I20" s="19">
-        <f t="shared" si="5"/>
-        <v>6405750</v>
-      </c>
-      <c r="J20" s="19">
-        <f t="shared" si="5"/>
-        <v>6405750</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="23">
-        <f>SUM(B14:B19)</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="25">
+      <c r="B11" s="29">
         <v>0.19</v>
       </c>
     </row>

</xml_diff>